<commit_message>
Practica#2 Cambio de contraseña antes de ingresar al sistema.
</commit_message>
<xml_diff>
--- a/betali_v2_asistencias/extras/temas.xlsx
+++ b/betali_v2_asistencias/extras/temas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\betali_v2_asistencias\extras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paperez\Desktop\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6615"/>
   </bookViews>
   <sheets>
     <sheet name="temas" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>id_tema</t>
   </si>
@@ -153,6 +153,9 @@
     <t>CHyP</t>
   </si>
   <si>
+    <t>$fff</t>
+  </si>
+  <si>
     <t>#ff9ff3</t>
   </si>
   <si>
@@ -160,26 +163,14 @@
   </si>
   <si>
     <t>#222f3e</t>
-  </si>
-  <si>
-    <t>Cool</t>
-  </si>
-  <si>
-    <t>#6D214F</t>
-  </si>
-  <si>
-    <t>#2f3542</t>
-  </si>
-  <si>
-    <t>#5758BB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -213,7 +204,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,16 +772,16 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="2">
         <v>43921</v>
@@ -799,35 +790,6 @@
         <v>0.55267361111111113</v>
       </c>
       <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="2">
-        <v>43921</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.70174768518518515</v>
-      </c>
-      <c r="I11">
         <v>1</v>
       </c>
     </row>

</xml_diff>